<commit_message>
modified:   Beilage_Verfuegung_per_Kreditor.xlsx     	modified:   PythonApplication4.py
</commit_message>
<xml_diff>
--- a/Beilage_Verfuegung_per_Kreditor.xlsx
+++ b/Beilage_Verfuegung_per_Kreditor.xlsx
@@ -49,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -62,10 +62,6 @@
     </font>
     <font>
       <i val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="4">
@@ -88,7 +84,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -100,18 +96,11 @@
       <bottom style="thin"/>
     </border>
     <border/>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -177,16 +166,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6816,7 +6795,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:H28"/>
+  <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7313,46 +7292,7 @@
       <c r="G25" s="3" t="n"/>
       <c r="H25" s="3" t="n"/>
     </row>
-    <row r="26">
-      <c r="A26" s="24" t="inlineStr">
-        <is>
-          <t>Begründungen (NA15)</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>ER Nr.</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="inlineStr">
-        <is>
-          <t>Begründung</t>
-        </is>
-      </c>
-      <c r="C27" s="25" t="n"/>
-      <c r="D27" s="25" t="n"/>
-      <c r="E27" s="25" t="n"/>
-      <c r="F27" s="25" t="n"/>
-    </row>
-    <row r="28" ht="15" customHeight="1">
-      <c r="A28" s="26" t="inlineStr">
-        <is>
-          <t>963040.0</t>
-        </is>
-      </c>
-      <c r="B28" s="27" t="inlineStr">
-        <is>
-          <t>Anderes</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="1" header="0.3" footer="0.5"/>
   <pageSetup orientation="landscape" paperSize="9" fitToHeight="0" fitToWidth="1"/>
   <headerFooter>

</xml_diff>